<commit_message>
students summary, timeout quiz
</commit_message>
<xml_diff>
--- a/DATABASE_TEMPLATES/UPLOAD_QUESTIONS_template_2.xlsx
+++ b/DATABASE_TEMPLATES/UPLOAD_QUESTIONS_template_2.xlsx
@@ -1231,6 +1231,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1519,10 +1520,20 @@
   <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H81"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="111.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="61.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="46.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="41.72"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1550,7 +1561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -2070,7 +2081,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
@@ -2096,7 +2107,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="305.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
@@ -2122,7 +2133,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="318.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
@@ -2148,7 +2159,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
@@ -2174,7 +2185,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
@@ -2200,7 +2211,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
@@ -2226,7 +2237,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
@@ -2252,7 +2263,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="267.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
@@ -2278,7 +2289,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
@@ -2304,7 +2315,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
@@ -2330,7 +2341,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="242.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
@@ -2356,7 +2367,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
@@ -2382,7 +2393,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
@@ -2408,7 +2419,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
@@ -2460,7 +2471,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
@@ -2512,7 +2523,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
@@ -2538,7 +2549,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
@@ -2564,7 +2575,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
@@ -2590,7 +2601,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
@@ -2616,7 +2627,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
@@ -2642,7 +2653,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="166.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
@@ -2668,7 +2679,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
@@ -2694,7 +2705,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
@@ -2720,7 +2731,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
@@ -2746,7 +2757,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
@@ -2772,7 +2783,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
@@ -2798,7 +2809,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
@@ -2824,7 +2835,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
@@ -2850,7 +2861,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>51</v>
       </c>
@@ -2876,7 +2887,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>52</v>
       </c>
@@ -2902,7 +2913,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="166.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>53</v>
       </c>
@@ -2928,7 +2939,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>54</v>
       </c>
@@ -2954,7 +2965,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>55</v>
       </c>
@@ -2980,7 +2991,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>56</v>
       </c>
@@ -3006,7 +3017,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>57</v>
       </c>
@@ -3032,7 +3043,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>58</v>
       </c>
@@ -3058,7 +3069,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>59</v>
       </c>
@@ -3084,7 +3095,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>60</v>
       </c>
@@ -3110,7 +3121,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>61</v>
       </c>
@@ -3136,7 +3147,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>62</v>
       </c>
@@ -3162,7 +3173,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>63</v>
       </c>
@@ -3188,7 +3199,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="217.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>64</v>
       </c>
@@ -3214,7 +3225,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>65</v>
       </c>
@@ -3240,7 +3251,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>66</v>
       </c>
@@ -3266,7 +3277,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>67</v>
       </c>
@@ -3292,7 +3303,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>68</v>
       </c>
@@ -3318,7 +3329,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>69</v>
       </c>
@@ -3344,7 +3355,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>70</v>
       </c>
@@ -3370,7 +3381,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>71</v>
       </c>
@@ -3396,7 +3407,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>72</v>
       </c>
@@ -3422,7 +3433,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>73</v>
       </c>
@@ -3448,7 +3459,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>74</v>
       </c>
@@ -3474,7 +3485,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>75</v>
       </c>
@@ -3500,7 +3511,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>76</v>
       </c>
@@ -3526,7 +3537,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>77</v>
       </c>
@@ -3552,7 +3563,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>78</v>
       </c>
@@ -3578,7 +3589,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <v>79</v>
       </c>
@@ -3604,7 +3615,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
         <v>80</v>
       </c>

</xml_diff>